<commit_message>
lesson $5 video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t xml:space="preserve">Java Basics – Data types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/CU-b7QVRpf0</t>
   </si>
   <si>
     <t xml:space="preserve">Java Basics – Operations</t>
@@ -546,17 +549,17 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="61.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="61.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="7.63"/>
   </cols>
   <sheetData>
@@ -1136,7 +1139,9 @@
       <c r="E16" s="17" t="n">
         <v>44163</v>
       </c>
-      <c r="F16" s="13"/>
+      <c r="F16" s="13" t="s">
+        <v>34</v>
+      </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -1164,7 +1169,7 @@
         <v>6</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D17" s="10" t="n">
         <v>2</v>
@@ -1200,7 +1205,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D18" s="10" t="n">
         <v>2</v>
@@ -1236,7 +1241,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D19" s="10" t="n">
         <v>2</v>
@@ -1269,7 +1274,7 @@
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="14"/>
       <c r="B20" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C20" s="22"/>
       <c r="D20" s="10"/>

</xml_diff>

<commit_message>
lesson #6 lesson video record uploaded to youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t xml:space="preserve">Java Basics – Operations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/Ejus0S8b4jU</t>
   </si>
   <si>
     <t xml:space="preserve">Java Basics – Conditions</t>
@@ -549,10 +552,10 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -1177,7 +1180,9 @@
       <c r="E17" s="17" t="n">
         <v>44167</v>
       </c>
-      <c r="F17" s="13"/>
+      <c r="F17" s="13" t="s">
+        <v>36</v>
+      </c>
       <c r="G17" s="4"/>
       <c r="H17" s="29"/>
       <c r="I17" s="4"/>
@@ -1205,7 +1210,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D18" s="10" t="n">
         <v>2</v>
@@ -1241,7 +1246,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D19" s="10" t="n">
         <v>2</v>
@@ -1274,7 +1279,7 @@
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="14"/>
       <c r="B20" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C20" s="22"/>
       <c r="D20" s="10"/>

</xml_diff>

<commit_message>
lesson #7 lesson video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -93,7 +93,7 @@
     <t xml:space="preserve">Final Exam</t>
   </si>
   <si>
-    <t xml:space="preserve">final exam here</t>
+    <t xml:space="preserve">final exam #1 here</t>
   </si>
   <si>
     <t xml:space="preserve">B. Intro to Prog</t>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t xml:space="preserve">Java Basics – Conditions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/4eaw1bZxdbc</t>
   </si>
   <si>
     <t xml:space="preserve">Java Basics – Loops</t>
@@ -551,11 +554,11 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -1218,7 +1221,9 @@
       <c r="E18" s="17" t="n">
         <v>44170</v>
       </c>
-      <c r="F18" s="13"/>
+      <c r="F18" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -1246,7 +1251,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D19" s="10" t="n">
         <v>2</v>
@@ -1279,7 +1284,7 @@
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="14"/>
       <c r="B20" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C20" s="22"/>
       <c r="D20" s="10"/>

</xml_diff>

<commit_message>
lesson 08 video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -149,7 +149,13 @@
     <t xml:space="preserve">Java Basics – Loops</t>
   </si>
   <si>
+    <t xml:space="preserve">https://youtu.be/OpAN6YuFids</t>
+  </si>
+  <si>
     <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java Basics – Loops – Practice</t>
   </si>
 </sst>
 </file>
@@ -555,10 +561,10 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -1259,7 +1265,9 @@
       <c r="E19" s="17" t="n">
         <v>44174</v>
       </c>
-      <c r="F19" s="13"/>
+      <c r="F19" s="13" t="s">
+        <v>40</v>
+      </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
@@ -1284,11 +1292,8 @@
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="14"/>
       <c r="B20" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="17"/>
       <c r="F20" s="13"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -1313,10 +1318,18 @@
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="14"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="17"/>
+      <c r="B21" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" s="17" t="n">
+        <v>44177</v>
+      </c>
       <c r="F21" s="13"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -1341,11 +1354,13 @@
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="4"/>
+      <c r="B22" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="13"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -1369,11 +1384,13 @@
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="4"/>
+      <c r="B23" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="C23" s="22"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="13"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
@@ -1397,11 +1414,13 @@
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="4"/>
+      <c r="B24" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="C24" s="22"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="13"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
@@ -1425,11 +1444,13 @@
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="4"/>
+      <c r="B25" s="10" t="n">
+        <v>5</v>
+      </c>
+      <c r="C25" s="22"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="13"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
@@ -1453,11 +1474,13 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="4"/>
+      <c r="B26" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="C26" s="22"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="13"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
@@ -1481,10 +1504,13 @@
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="5"/>
+      <c r="B27" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="13"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
@@ -1508,11 +1534,13 @@
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="4"/>
+      <c r="B28" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C28" s="22"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="13"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>

</xml_diff>

<commit_message>
lesson 09 video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -152,10 +152,13 @@
     <t xml:space="preserve">https://youtu.be/OpAN6YuFids</t>
   </si>
   <si>
-    <t xml:space="preserve">-</t>
+    <t xml:space="preserve">Java Basics – Loops – Practice</t>
   </si>
   <si>
-    <t xml:space="preserve">Java Basics – Loops – Practice</t>
+    <t xml:space="preserve">https://youtu.be/cnaRJ5bY3Wo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methods</t>
   </si>
 </sst>
 </file>
@@ -360,7 +363,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -398,7 +401,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -415,10 +418,6 @@
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -469,6 +468,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -479,6 +482,10 @@
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -560,11 +567,11 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -716,7 +723,7 @@
       <c r="Z4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="10" t="n">
         <f aca="false">B4+1</f>
         <v>1</v>
@@ -727,7 +734,7 @@
       <c r="D5" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E5" s="15" t="n">
+      <c r="E5" s="14" t="n">
         <v>44117</v>
       </c>
       <c r="F5" s="13" t="s">
@@ -755,21 +762,21 @@
       <c r="Z5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="10" t="n">
         <f aca="false">B5+1</f>
         <v>2</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E6" s="17" t="n">
+      <c r="E6" s="16" t="n">
         <v>44121</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="17" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="4"/>
@@ -794,7 +801,7 @@
       <c r="Z6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="10" t="n">
         <f aca="false">B6+1</f>
         <v>3</v>
@@ -805,10 +812,10 @@
       <c r="D7" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E7" s="17" t="n">
+      <c r="E7" s="16" t="n">
         <v>44124</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="17" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="4"/>
@@ -833,7 +840,7 @@
       <c r="Z7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="10" t="n">
         <f aca="false">B7+1</f>
         <v>4</v>
@@ -844,10 +851,10 @@
       <c r="D8" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E8" s="17" t="n">
+      <c r="E8" s="16" t="n">
         <v>44128</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="17" t="s">
         <v>18</v>
       </c>
       <c r="G8" s="4"/>
@@ -872,25 +879,25 @@
       <c r="Z8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="10" t="n">
         <f aca="false">B8+1</f>
         <v>5</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E9" s="17" t="n">
+      <c r="E9" s="16" t="n">
         <v>44131</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="19" t="s">
         <v>20</v>
       </c>
       <c r="G9" s="4"/>
-      <c r="H9" s="21"/>
+      <c r="H9" s="20"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -911,21 +918,21 @@
       <c r="Z9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="10" t="n">
         <f aca="false">B9+1</f>
         <v>6</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E10" s="17" t="n">
+      <c r="E10" s="16" t="n">
         <v>44135</v>
       </c>
-      <c r="F10" s="20"/>
+      <c r="F10" s="19"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -948,18 +955,18 @@
       <c r="Z10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14"/>
-      <c r="B11" s="23" t="n">
+      <c r="A11" s="9"/>
+      <c r="B11" s="22" t="n">
         <v>7</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="25" t="n">
+      <c r="D11" s="22"/>
+      <c r="E11" s="24" t="n">
         <v>44138</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="25" t="s">
         <v>23</v>
       </c>
       <c r="G11" s="4"/>
@@ -984,19 +991,19 @@
       <c r="Z11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="26" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="21" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E12" s="17" t="n">
+      <c r="E12" s="16" t="n">
         <v>44142</v>
       </c>
       <c r="F12" s="27" t="s">
@@ -1024,17 +1031,17 @@
       <c r="Z12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="21" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E13" s="17" t="n">
+      <c r="E13" s="16" t="n">
         <v>44150</v>
       </c>
       <c r="F13" s="27" t="s">
@@ -1062,20 +1069,20 @@
       <c r="Z13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D14" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E14" s="17" t="n">
+      <c r="E14" s="16" t="n">
         <v>44156</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="19" t="s">
         <v>30</v>
       </c>
       <c r="G14" s="4"/>
@@ -1100,17 +1107,17 @@
       <c r="Z14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="21" t="s">
         <v>31</v>
       </c>
       <c r="D15" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E15" s="17" t="n">
+      <c r="E15" s="16" t="n">
         <v>44160</v>
       </c>
       <c r="F15" s="28" t="s">
@@ -1138,17 +1145,17 @@
       <c r="Z15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="21" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E16" s="17" t="n">
+      <c r="E16" s="16" t="n">
         <v>44163</v>
       </c>
       <c r="F16" s="13" t="s">
@@ -1176,17 +1183,17 @@
       <c r="Z16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="21" t="s">
         <v>35</v>
       </c>
       <c r="D17" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E17" s="17" t="n">
+      <c r="E17" s="16" t="n">
         <v>44167</v>
       </c>
       <c r="F17" s="13" t="s">
@@ -1214,17 +1221,17 @@
       <c r="Z17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="21" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E18" s="17" t="n">
+      <c r="E18" s="16" t="n">
         <v>44170</v>
       </c>
       <c r="F18" s="13" t="s">
@@ -1252,17 +1259,17 @@
       <c r="Z18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="21" t="s">
         <v>39</v>
       </c>
       <c r="D19" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E19" s="17" t="n">
+      <c r="E19" s="16" t="n">
         <v>44174</v>
       </c>
       <c r="F19" s="13" t="s">
@@ -1290,11 +1297,22 @@
       <c r="Z19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14"/>
-      <c r="B20" s="10" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C20" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="13"/>
+      <c r="D20" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" s="16" t="n">
+        <v>44177</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
@@ -1317,20 +1335,8 @@
       <c r="Z20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14"/>
-      <c r="B21" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="E21" s="17" t="n">
-        <v>44177</v>
-      </c>
-      <c r="F21" s="13"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="10"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -1355,11 +1361,17 @@
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="4"/>
       <c r="B22" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="17"/>
+      <c r="E22" s="16" t="n">
+        <v>44181</v>
+      </c>
       <c r="F22" s="13"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -1385,11 +1397,11 @@
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
       <c r="B23" s="10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
-      <c r="C23" s="22"/>
+      <c r="C23" s="21"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="17"/>
+      <c r="E23" s="16"/>
       <c r="F23" s="13"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -1415,11 +1427,11 @@
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
       <c r="B24" s="10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
-      <c r="C24" s="22"/>
+      <c r="C24" s="21"/>
       <c r="D24" s="10"/>
-      <c r="E24" s="17"/>
+      <c r="E24" s="16"/>
       <c r="F24" s="13"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -1445,11 +1457,11 @@
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>
       <c r="B25" s="10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
-      <c r="C25" s="22"/>
+      <c r="C25" s="21"/>
       <c r="D25" s="10"/>
-      <c r="E25" s="17"/>
+      <c r="E25" s="16"/>
       <c r="F25" s="13"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -1475,11 +1487,11 @@
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
       <c r="B26" s="10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
-      <c r="C26" s="22"/>
+      <c r="C26" s="21"/>
       <c r="D26" s="10"/>
-      <c r="E26" s="17"/>
+      <c r="E26" s="16"/>
       <c r="F26" s="13"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -1505,11 +1517,11 @@
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
       <c r="B27" s="10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
-      <c r="C27" s="22"/>
+      <c r="C27" s="21"/>
       <c r="D27" s="10"/>
-      <c r="E27" s="17"/>
+      <c r="E27" s="16"/>
       <c r="F27" s="13"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -1535,11 +1547,11 @@
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4"/>
       <c r="B28" s="10" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
-      <c r="C28" s="22"/>
+      <c r="C28" s="21"/>
       <c r="D28" s="10"/>
-      <c r="E28" s="17"/>
+      <c r="E28" s="16"/>
       <c r="F28" s="13"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -28750,8 +28762,10 @@
       <c r="Z999" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
+    <mergeCell ref="A4:A11"/>
     <mergeCell ref="F9:F10"/>
+    <mergeCell ref="A12:A20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" display="https://youtu.be/N5L2Jc5uzmU"/>
@@ -28762,6 +28776,7 @@
     <hyperlink ref="F13" r:id="rId6" display="part1: https://youtu.be/irIslLEDWoE&#10;part2: https://youtu.be/hyHVF0DS7B8&#10;part3: https://youtu.be/I8gxXlg5_YU"/>
     <hyperlink ref="F14" r:id="rId7" display="part1: https://youtu.be/jqDT7u_Wab0&#10;part2: https://youtu.be/jKJ6tknff5A"/>
     <hyperlink ref="F15" r:id="rId8" display="https://youtu.be/VwGZValoyfI"/>
+    <hyperlink ref="F20" r:id="rId9" display="https://youtu.be/cnaRJ5bY3Wo"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson 09 class code added
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -568,10 +568,10 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>

</xml_diff>

<commit_message>
lesson 10 video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t xml:space="preserve">Methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrays</t>
   </si>
 </sst>
 </file>
@@ -561,17 +564,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -1399,9 +1402,15 @@
       <c r="B23" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="16"/>
+      <c r="C23" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" s="16" t="n">
+        <v>44184</v>
+      </c>
       <c r="F23" s="13"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>

</xml_diff>

<commit_message>
lesson 12 lesson code
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t xml:space="preserve">Arrays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/S6AdxJimaR8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrays #2</t>
   </si>
 </sst>
 </file>
@@ -573,11 +579,11 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -1416,7 +1422,9 @@
       <c r="E23" s="16" t="n">
         <v>44184</v>
       </c>
-      <c r="F23" s="13"/>
+      <c r="F23" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
@@ -1443,9 +1451,15 @@
       <c r="B24" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="16"/>
+      <c r="C24" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E24" s="16" t="n">
+        <v>44188</v>
+      </c>
       <c r="F24" s="13"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>

</xml_diff>

<commit_message>
lesson 12 video record on youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -171,6 +171,12 @@
   </si>
   <si>
     <t xml:space="preserve">Arrays #2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/dhSEoY8BHgI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrays #3</t>
   </si>
 </sst>
 </file>
@@ -580,10 +586,10 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -1460,7 +1466,9 @@
       <c r="E24" s="16" t="n">
         <v>44188</v>
       </c>
-      <c r="F24" s="13"/>
+      <c r="F24" s="13" t="s">
+        <v>48</v>
+      </c>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
@@ -1487,9 +1495,15 @@
       <c r="B25" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="16"/>
+      <c r="C25" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E25" s="16" t="n">
+        <v>44191</v>
+      </c>
       <c r="F25" s="13"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>

</xml_diff>

<commit_message>
lesson 13 video record on youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -177,6 +177,12 @@
   </si>
   <si>
     <t xml:space="preserve">Arrays #3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/9zs9DaszFsc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String intro</t>
   </si>
 </sst>
 </file>
@@ -585,11 +591,11 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -1504,7 +1510,9 @@
       <c r="E25" s="16" t="n">
         <v>44191</v>
       </c>
-      <c r="F25" s="13"/>
+      <c r="F25" s="13" t="s">
+        <v>50</v>
+      </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
@@ -1531,9 +1539,15 @@
       <c r="B26" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="16"/>
+      <c r="C26" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E26" s="16" t="n">
+        <v>44202</v>
+      </c>
       <c r="F26" s="13"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -28819,6 +28833,7 @@
     <hyperlink ref="F14" r:id="rId7" display="part1: https://youtu.be/jqDT7u_Wab0&#10;part2: https://youtu.be/jKJ6tknff5A"/>
     <hyperlink ref="F15" r:id="rId8" display="https://youtu.be/VwGZValoyfI"/>
     <hyperlink ref="F20" r:id="rId9" display="https://youtu.be/cnaRJ5bY3Wo"/>
+    <hyperlink ref="F25" r:id="rId10" display="https://youtu.be/9zs9DaszFsc"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson 14 video record upload into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -184,6 +184,34 @@
   <si>
     <t xml:space="preserve">String intro</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color rgb="FF0563C1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Part #1: https://youtu.be/DcA2l_JuptA 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color rgb="FF0563C1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Part #2: https://youtu.be/Bh46FyQNxbk
+Part #3: https://youtu.be/HaiIudq5uG4</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Memory Management in java (jvm)</t>
+  </si>
 </sst>
 </file>
 
@@ -193,7 +221,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -310,6 +338,13 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -387,7 +422,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -512,6 +547,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,10 +635,10 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -1534,12 +1577,12 @@
       <c r="Y25" s="4"/>
       <c r="Z25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="41.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
       <c r="B26" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="31" t="s">
         <v>51</v>
       </c>
       <c r="D26" s="10" t="n">
@@ -1548,7 +1591,9 @@
       <c r="E26" s="16" t="n">
         <v>44202</v>
       </c>
-      <c r="F26" s="13"/>
+      <c r="F26" s="32" t="s">
+        <v>52</v>
+      </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
@@ -1575,9 +1620,15 @@
       <c r="B27" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="16"/>
+      <c r="C27" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" s="16" t="n">
+        <v>44205</v>
+      </c>
       <c r="F27" s="13"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -28834,6 +28885,7 @@
     <hyperlink ref="F15" r:id="rId8" display="https://youtu.be/VwGZValoyfI"/>
     <hyperlink ref="F20" r:id="rId9" display="https://youtu.be/cnaRJ5bY3Wo"/>
     <hyperlink ref="F25" r:id="rId10" display="https://youtu.be/9zs9DaszFsc"/>
+    <hyperlink ref="F26" r:id="rId11" display="https://youtu.be/HaiIudq5uG4"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #15 lesson video record in youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -185,32 +185,17 @@
     <t xml:space="preserve">String intro</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="11"/>
-        <color rgb="FF0563C1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Part #1: https://youtu.be/DcA2l_JuptA 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="11"/>
-        <color rgb="FF0563C1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Part #2: https://youtu.be/Bh46FyQNxbk
-Part #3: https://youtu.be/HaiIudq5uG4</t>
-    </r>
+    <t xml:space="preserve">Part #1: https://youtu.be/DcA2l_JuptA 
+Part #2: https://youtu.be/Bh46FyQNxbk 
+Part #3: https://youtu.be/HaiIudq5uG4 </t>
   </si>
   <si>
     <t xml:space="preserve">Memory Management in java (jvm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part #1: https://youtu.be/qoLLV7zGCNw
+Part #2: https://youtu.be/Ojr54_tl_eE
+Part #3: https://youtu.be/fcLU3d7mW4M </t>
   </si>
 </sst>
 </file>
@@ -221,7 +206,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -337,13 +322,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF0563C1"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -634,11 +612,11 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B18" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -1615,12 +1593,12 @@
       <c r="Y26" s="4"/>
       <c r="Z26" s="4"/>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
       <c r="B27" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="31" t="s">
         <v>53</v>
       </c>
       <c r="D27" s="10" t="n">
@@ -1629,7 +1607,9 @@
       <c r="E27" s="16" t="n">
         <v>44205</v>
       </c>
-      <c r="F27" s="13"/>
+      <c r="F27" s="32" t="s">
+        <v>54</v>
+      </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
@@ -28885,7 +28865,6 @@
     <hyperlink ref="F15" r:id="rId8" display="https://youtu.be/VwGZValoyfI"/>
     <hyperlink ref="F20" r:id="rId9" display="https://youtu.be/cnaRJ5bY3Wo"/>
     <hyperlink ref="F25" r:id="rId10" display="https://youtu.be/9zs9DaszFsc"/>
-    <hyperlink ref="F26" r:id="rId11" display="https://youtu.be/HaiIudq5uG4"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #16 course syllabus updated
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -198,7 +198,22 @@
 Part #3: https://youtu.be/fcLU3d7mW4M </t>
   </si>
   <si>
+    <t xml:space="preserve">https://youtu.be/VYnEWiP1fu0 </t>
+  </si>
+  <si>
     <t xml:space="preserve">Full recap and practice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OOP #1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OOP #2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OOP #3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OOP #4</t>
   </si>
 </sst>
 </file>
@@ -629,11 +644,11 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.4765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -1662,7 +1677,9 @@
       <c r="E28" s="17" t="n">
         <v>44209</v>
       </c>
-      <c r="F28" s="14"/>
+      <c r="F28" s="14" t="s">
+        <v>55</v>
+      </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
@@ -1690,7 +1707,7 @@
         <v>8</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D29" s="12" t="n">
         <v>2</v>
@@ -1750,11 +1767,17 @@
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="4"/>
+      <c r="B31" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E31" s="17"/>
+      <c r="F31" s="14"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
@@ -1778,11 +1801,17 @@
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="4"/>
+      <c r="B32" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E32" s="17"/>
+      <c r="F32" s="14"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
@@ -1806,11 +1835,17 @@
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="4"/>
+      <c r="B33" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E33" s="17"/>
+      <c r="F33" s="14"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
@@ -1834,11 +1869,17 @@
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="4"/>
+      <c r="B34" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E34" s="17"/>
+      <c r="F34" s="14"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
@@ -1862,11 +1903,15 @@
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="4"/>
+      <c r="B35" s="12" t="n">
+        <v>5</v>
+      </c>
+      <c r="C35" s="33"/>
+      <c r="D35" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E35" s="17"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
@@ -1890,11 +1935,15 @@
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="4"/>
+      <c r="B36" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="C36" s="33"/>
+      <c r="D36" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E36" s="17"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
@@ -1918,11 +1967,15 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="4"/>
+      <c r="B37" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="C37" s="33"/>
+      <c r="D37" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E37" s="17"/>
+      <c r="F37" s="14"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
@@ -1946,11 +1999,15 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="4"/>
+      <c r="B38" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C38" s="22"/>
+      <c r="D38" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E38" s="17"/>
+      <c r="F38" s="14"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>

</xml_diff>

<commit_message>
lesson #18 video record uploaded into yourube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -202,6 +202,11 @@
   </si>
   <si>
     <t xml:space="preserve">Full recap and practice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part #1: https://youtu.be/TVo1nFW_cew
+Part #2: https://youtu.be/59Jgz52nctg
+Part #3: https://youtu.be/bISInVBVX6A</t>
   </si>
   <si>
     <t xml:space="preserve">OOP #1</t>
@@ -645,10 +650,10 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
+      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -1701,12 +1706,12 @@
       <c r="Y28" s="4"/>
       <c r="Z28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="41.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4"/>
       <c r="B29" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="33" t="s">
         <v>56</v>
       </c>
       <c r="D29" s="12" t="n">
@@ -1715,7 +1720,9 @@
       <c r="E29" s="17" t="n">
         <v>44212</v>
       </c>
-      <c r="F29" s="14"/>
+      <c r="F29" s="34" t="s">
+        <v>57</v>
+      </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
@@ -1771,7 +1778,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D31" s="12" t="n">
         <v>2</v>
@@ -1805,7 +1812,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D32" s="12" t="n">
         <v>2</v>
@@ -1839,7 +1846,7 @@
         <v>3</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D33" s="12" t="n">
         <v>2</v>
@@ -1873,7 +1880,7 @@
         <v>4</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D34" s="12" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
lesson #18 video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -210,6 +210,11 @@
   </si>
   <si>
     <t xml:space="preserve">OOP #1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part #1: https://youtu.be/ubHNRSLfOPU
+Part #2: https://youtu.be/6FkknwgD7zI
+Part #3: https://youtu.be/-ovFX92_aes</t>
   </si>
   <si>
     <t xml:space="preserve">OOP #2</t>
@@ -429,7 +434,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -570,6 +575,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,10 +659,10 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
+      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -1772,39 +1781,43 @@
       <c r="Y30" s="4"/>
       <c r="Z30" s="4"/>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4"/>
+    <row r="31" s="35" customFormat="true" ht="41.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="21"/>
       <c r="B31" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="33" t="s">
         <v>58</v>
       </c>
       <c r="D31" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="E31" s="17"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
-      <c r="U31" s="4"/>
-      <c r="V31" s="4"/>
-      <c r="W31" s="4"/>
-      <c r="X31" s="4"/>
-      <c r="Y31" s="4"/>
-      <c r="Z31" s="4"/>
+      <c r="E31" s="17" t="n">
+        <v>44216</v>
+      </c>
+      <c r="F31" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="21"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="21"/>
+      <c r="U31" s="21"/>
+      <c r="V31" s="21"/>
+      <c r="W31" s="21"/>
+      <c r="X31" s="21"/>
+      <c r="Y31" s="21"/>
+      <c r="Z31" s="21"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="4"/>
@@ -1812,7 +1825,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D32" s="12" t="n">
         <v>2</v>
@@ -1846,7 +1859,7 @@
         <v>3</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D33" s="12" t="n">
         <v>2</v>
@@ -1880,7 +1893,7 @@
         <v>4</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D34" s="12" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
course syllabus polished a bit
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -659,10 +659,10 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
+      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -1830,7 +1830,9 @@
       <c r="D32" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="E32" s="17"/>
+      <c r="E32" s="17" t="n">
+        <v>44219</v>
+      </c>
       <c r="F32" s="14"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -1864,7 +1866,9 @@
       <c r="D33" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="E33" s="17"/>
+      <c r="E33" s="17" t="n">
+        <v>44223</v>
+      </c>
       <c r="F33" s="14"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
@@ -1898,7 +1902,9 @@
       <c r="D34" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="E34" s="17"/>
+      <c r="E34" s="17" t="n">
+        <v>44226</v>
+      </c>
       <c r="F34" s="14"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>

</xml_diff>

<commit_message>
lesson #19 video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -218,6 +218,11 @@
   </si>
   <si>
     <t xml:space="preserve">OOP #2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part #1: https://youtu.be/7uTpemicD8I
+Part #2: https://youtu.be/GOgX4U85ge8
+Part #3: https://youtu.be/J05isj-ABFc</t>
   </si>
   <si>
     <t xml:space="preserve">OOP #3</t>
@@ -659,10 +664,10 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -1819,12 +1824,12 @@
       <c r="Y31" s="21"/>
       <c r="Z31" s="21"/>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4"/>
+    <row r="32" s="35" customFormat="true" ht="41.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="21"/>
       <c r="B32" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="33" t="s">
         <v>60</v>
       </c>
       <c r="D32" s="12" t="n">
@@ -1833,27 +1838,29 @@
       <c r="E32" s="17" t="n">
         <v>44219</v>
       </c>
-      <c r="F32" s="14"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
-      <c r="U32" s="4"/>
-      <c r="V32" s="4"/>
-      <c r="W32" s="4"/>
-      <c r="X32" s="4"/>
-      <c r="Y32" s="4"/>
-      <c r="Z32" s="4"/>
+      <c r="F32" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="21"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="21"/>
+      <c r="U32" s="21"/>
+      <c r="V32" s="21"/>
+      <c r="W32" s="21"/>
+      <c r="X32" s="21"/>
+      <c r="Y32" s="21"/>
+      <c r="Z32" s="21"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="4"/>
@@ -1861,7 +1868,7 @@
         <v>3</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D33" s="12" t="n">
         <v>2</v>
@@ -1897,7 +1904,7 @@
         <v>4</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D34" s="12" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
lesson #20 lesson code and slide attached
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -228,7 +228,15 @@
     <t xml:space="preserve">OOP #3</t>
   </si>
   <si>
+    <t xml:space="preserve">Part #1: 
+Part #2: 
+Part #3: </t>
+  </si>
+  <si>
     <t xml:space="preserve">OOP #4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OOP #5</t>
   </si>
 </sst>
 </file>
@@ -664,10 +672,10 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
+      <selection pane="topLeft" activeCell="G33" activeCellId="0" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -1862,12 +1870,12 @@
       <c r="Y32" s="21"/>
       <c r="Z32" s="21"/>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4"/>
+    <row r="33" s="35" customFormat="true" ht="41.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="21"/>
       <c r="B33" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="33" t="s">
         <v>62</v>
       </c>
       <c r="D33" s="12" t="n">
@@ -1876,27 +1884,29 @@
       <c r="E33" s="17" t="n">
         <v>44223</v>
       </c>
-      <c r="F33" s="14"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
-      <c r="U33" s="4"/>
-      <c r="V33" s="4"/>
-      <c r="W33" s="4"/>
-      <c r="X33" s="4"/>
-      <c r="Y33" s="4"/>
-      <c r="Z33" s="4"/>
+      <c r="F33" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="21"/>
+      <c r="O33" s="21"/>
+      <c r="P33" s="21"/>
+      <c r="Q33" s="21"/>
+      <c r="R33" s="21"/>
+      <c r="S33" s="21"/>
+      <c r="T33" s="21"/>
+      <c r="U33" s="21"/>
+      <c r="V33" s="21"/>
+      <c r="W33" s="21"/>
+      <c r="X33" s="21"/>
+      <c r="Y33" s="21"/>
+      <c r="Z33" s="21"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
@@ -1904,7 +1914,7 @@
         <v>4</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D34" s="12" t="n">
         <v>2</v>
@@ -1939,11 +1949,15 @@
       <c r="B35" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="C35" s="33"/>
+      <c r="C35" s="22" t="s">
+        <v>65</v>
+      </c>
       <c r="D35" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="E35" s="17"/>
+      <c r="E35" s="17" t="n">
+        <v>44230</v>
+      </c>
       <c r="F35" s="34"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>

</xml_diff>

<commit_message>
lesson #20 video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -228,9 +228,9 @@
     <t xml:space="preserve">OOP #3</t>
   </si>
   <si>
-    <t xml:space="preserve">Part #1: 
-Part #2: 
-Part #3: </t>
+    <t xml:space="preserve">Part #1: https://youtu.be/btgFFWq-NWs
+Part #2: https://youtu.be/djhF8igWktA
+Part #3: https://youtu.be/MKrUA6DWMU8</t>
   </si>
   <si>
     <t xml:space="preserve">OOP #4</t>
@@ -672,10 +672,10 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G33" activeCellId="0" sqref="G33"/>
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.41015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>

</xml_diff>

<commit_message>
lesson #21 video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -236,7 +236,39 @@
     <t xml:space="preserve">OOP #4</t>
   </si>
   <si>
-    <t xml:space="preserve">OOP #5</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color rgb="FF0563C1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Part #1: </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color rgb="FF0563C1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">https://youtu.be/M3gRRFvtmDY
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color rgb="FF0563C1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Part #2: https://youtu.be/gDldNTd99bI</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -247,7 +279,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -363,6 +395,13 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -671,11 +710,11 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.41015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.40234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -1908,7 +1947,7 @@
       <c r="Y33" s="21"/>
       <c r="Z33" s="21"/>
     </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
       <c r="B34" s="12" t="n">
         <v>4</v>
@@ -1922,7 +1961,9 @@
       <c r="E34" s="17" t="n">
         <v>44226</v>
       </c>
-      <c r="F34" s="14"/>
+      <c r="F34" s="34" t="s">
+        <v>65</v>
+      </c>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
@@ -1949,15 +1990,9 @@
       <c r="B35" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="C35" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="D35" s="12" t="n">
-        <v>2</v>
-      </c>
-      <c r="E35" s="17" t="n">
-        <v>44230</v>
-      </c>
+      <c r="C35" s="22"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="17"/>
       <c r="F35" s="34"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
@@ -1986,9 +2021,7 @@
         <v>6</v>
       </c>
       <c r="C36" s="33"/>
-      <c r="D36" s="12" t="n">
-        <v>2</v>
-      </c>
+      <c r="D36" s="12"/>
       <c r="E36" s="17"/>
       <c r="F36" s="34"/>
       <c r="G36" s="4"/>
@@ -2018,9 +2051,7 @@
         <v>7</v>
       </c>
       <c r="C37" s="33"/>
-      <c r="D37" s="12" t="n">
-        <v>2</v>
-      </c>
+      <c r="D37" s="12"/>
       <c r="E37" s="17"/>
       <c r="F37" s="14"/>
       <c r="G37" s="4"/>
@@ -2050,9 +2081,7 @@
         <v>8</v>
       </c>
       <c r="C38" s="22"/>
-      <c r="D38" s="12" t="n">
-        <v>2</v>
-      </c>
+      <c r="D38" s="12"/>
       <c r="E38" s="17"/>
       <c r="F38" s="14"/>
       <c r="G38" s="4"/>

</xml_diff>

<commit_message>
lesson #22 video record in youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -236,39 +236,19 @@
     <t xml:space="preserve">OOP #4</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="11"/>
-        <color rgb="FF0563C1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Part #1: </t>
-    </r>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="11"/>
-        <color rgb="FF0563C1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">https://youtu.be/M3gRRFvtmDY
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="11"/>
-        <color rgb="FF0563C1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Part #2: https://youtu.be/gDldNTd99bI</t>
-    </r>
+    <t xml:space="preserve">Part #1: https://youtu.be/M3gRRFvtmDY
+Part #2: https://youtu.be/gDldNTd99bI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OOP #5 – Abstraction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/3xcpCB8LbeQ
+https://youtu.be/9PIwgylR3BM
+https://youtu.be/AcUvMFY8KEg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OOP #6 – Interfaces</t>
   </si>
 </sst>
 </file>
@@ -279,7 +259,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -395,13 +375,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF0563C1"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -710,11 +683,11 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.40234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -1985,44 +1958,58 @@
       <c r="Y34" s="4"/>
       <c r="Z34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4"/>
+    <row r="35" s="35" customFormat="true" ht="41.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="21"/>
       <c r="B35" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
-      <c r="T35" s="4"/>
-      <c r="U35" s="4"/>
-      <c r="V35" s="4"/>
-      <c r="W35" s="4"/>
-      <c r="X35" s="4"/>
-      <c r="Y35" s="4"/>
-      <c r="Z35" s="4"/>
+      <c r="C35" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E35" s="17" t="n">
+        <v>44230</v>
+      </c>
+      <c r="F35" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="21"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="21"/>
+      <c r="P35" s="21"/>
+      <c r="Q35" s="21"/>
+      <c r="R35" s="21"/>
+      <c r="S35" s="21"/>
+      <c r="T35" s="21"/>
+      <c r="U35" s="21"/>
+      <c r="V35" s="21"/>
+      <c r="W35" s="21"/>
+      <c r="X35" s="21"/>
+      <c r="Y35" s="21"/>
+      <c r="Z35" s="21"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="4"/>
       <c r="B36" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="C36" s="33"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="17"/>
+      <c r="C36" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E36" s="17" t="n">
+        <v>44233</v>
+      </c>
       <c r="F36" s="34"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
@@ -29029,6 +29016,7 @@
     <hyperlink ref="F15" r:id="rId8" display="https://youtu.be/VwGZValoyfI"/>
     <hyperlink ref="F20" r:id="rId9" display="https://youtu.be/cnaRJ5bY3Wo"/>
     <hyperlink ref="F25" r:id="rId10" display="https://youtu.be/9zs9DaszFsc"/>
+    <hyperlink ref="F35" r:id="rId11" display="https://youtu.be/AcUvMFY8KEg"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #23 video record on youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -243,12 +243,15 @@
     <t xml:space="preserve">OOP #5 – Abstraction</t>
   </si>
   <si>
-    <t xml:space="preserve">https://youtu.be/3xcpCB8LbeQ
-https://youtu.be/9PIwgylR3BM
-https://youtu.be/AcUvMFY8KEg</t>
+    <t xml:space="preserve">1. https://youtu.be/3xcpCB8LbeQ
+2. https://youtu.be/9PIwgylR3BM
+3. https://youtu.be/AcUvMFY8KEg</t>
   </si>
   <si>
     <t xml:space="preserve">OOP #6 – Interfaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/tldgh05D1zc</t>
   </si>
 </sst>
 </file>
@@ -684,10 +687,10 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
+      <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.37109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -2010,7 +2013,9 @@
       <c r="E36" s="17" t="n">
         <v>44233</v>
       </c>
-      <c r="F36" s="34"/>
+      <c r="F36" s="34" t="s">
+        <v>69</v>
+      </c>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
@@ -29016,7 +29021,7 @@
     <hyperlink ref="F15" r:id="rId8" display="https://youtu.be/VwGZValoyfI"/>
     <hyperlink ref="F20" r:id="rId9" display="https://youtu.be/cnaRJ5bY3Wo"/>
     <hyperlink ref="F25" r:id="rId10" display="https://youtu.be/9zs9DaszFsc"/>
-    <hyperlink ref="F35" r:id="rId11" display="https://youtu.be/AcUvMFY8KEg"/>
+    <hyperlink ref="F36" r:id="rId11" display="https://youtu.be/tldgh05D1zc"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #24 lesson code attached
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://youtu.be/tldgh05D1zc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exceptions</t>
   </si>
 </sst>
 </file>
@@ -690,7 +693,7 @@
       <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.37109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.36328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -2042,9 +2045,15 @@
       <c r="B37" s="12" t="n">
         <v>7</v>
       </c>
-      <c r="C37" s="33"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="17"/>
+      <c r="C37" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E37" s="17" t="n">
+        <v>44237</v>
+      </c>
       <c r="F37" s="14"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>

</xml_diff>

<commit_message>
lesson #24 lesson video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -255,6 +255,12 @@
   </si>
   <si>
     <t xml:space="preserve">Exceptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/B7X01IIgi8Q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File IO</t>
   </si>
 </sst>
 </file>
@@ -690,10 +696,10 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
+      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.36328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.33984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -2054,7 +2060,9 @@
       <c r="E37" s="17" t="n">
         <v>44237</v>
       </c>
-      <c r="F37" s="14"/>
+      <c r="F37" s="14" t="s">
+        <v>71</v>
+      </c>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
@@ -2081,9 +2089,15 @@
       <c r="B38" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="C38" s="22"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="17"/>
+      <c r="C38" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E38" s="17" t="n">
+        <v>44242</v>
+      </c>
       <c r="F38" s="14"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
@@ -29031,6 +29045,7 @@
     <hyperlink ref="F20" r:id="rId9" display="https://youtu.be/cnaRJ5bY3Wo"/>
     <hyperlink ref="F25" r:id="rId10" display="https://youtu.be/9zs9DaszFsc"/>
     <hyperlink ref="F36" r:id="rId11" display="https://youtu.be/tldgh05D1zc"/>
+    <hyperlink ref="F37" r:id="rId12" display="https://youtu.be/B7X01IIgi8Q"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #27 video record on youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -273,6 +273,17 @@
     <t xml:space="preserve">1. https://youtu.be/KA5HBuESzkA
 2. https://youtu.be/T8WipvRMKQY
 3. https://youtu.be/JLnpYSM2HSM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step project #2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/7muiM7fBkxY
+https://youtu.be/XjTfFqC4pks
+https://youtu.be/LPpOp21JWPk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database #1</t>
   </si>
 </sst>
 </file>
@@ -685,14 +696,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
+      <selection pane="topLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2093,7 +2104,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="18" t="n">
-        <v>44242</v>
+        <v>44240</v>
       </c>
       <c r="F38" s="31" t="s">
         <v>73</v>
@@ -2159,7 +2170,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="18" t="n">
-        <v>44249</v>
+        <v>44247</v>
       </c>
       <c r="F40" s="31" t="s">
         <v>75</v>
@@ -2185,17 +2196,23 @@
       <c r="Y40" s="5"/>
       <c r="Z40" s="5"/>
     </row>
-    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="41.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5"/>
       <c r="B41" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="C41" s="21"/>
+      <c r="C41" s="21" t="s">
+        <v>76</v>
+      </c>
       <c r="D41" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="E41" s="18"/>
-      <c r="F41" s="31"/>
+      <c r="E41" s="18" t="n">
+        <v>44254</v>
+      </c>
+      <c r="F41" s="31" t="s">
+        <v>77</v>
+      </c>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
@@ -2222,11 +2239,15 @@
       <c r="B42" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="C42" s="21"/>
+      <c r="C42" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="D42" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="E42" s="18"/>
+      <c r="E42" s="18" t="n">
+        <v>44256</v>
+      </c>
       <c r="F42" s="31"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
@@ -29083,6 +29104,7 @@
     <hyperlink ref="F25" r:id="rId10" display="https://youtu.be/9zs9DaszFsc"/>
     <hyperlink ref="F36" r:id="rId11" display="https://youtu.be/tldgh05D1zc"/>
     <hyperlink ref="F37" r:id="rId12" display="https://youtu.be/B7X01IIgi8Q"/>
+    <hyperlink ref="F41" r:id="rId13" display="https://youtu.be/LPpOp21JWPk"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #28 video record on youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -284,6 +284,12 @@
   </si>
   <si>
     <t xml:space="preserve">Database #1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/faEWkrmhco8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database #2</t>
   </si>
 </sst>
 </file>
@@ -703,7 +709,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
+      <selection pane="topLeft" activeCell="F43" activeCellId="0" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2248,7 +2254,9 @@
       <c r="E42" s="18" t="n">
         <v>44256</v>
       </c>
-      <c r="F42" s="31"/>
+      <c r="F42" s="31" t="s">
+        <v>79</v>
+      </c>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
@@ -2275,11 +2283,15 @@
       <c r="B43" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="C43" s="21"/>
+      <c r="C43" s="21" t="s">
+        <v>80</v>
+      </c>
       <c r="D43" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="E43" s="18"/>
+      <c r="E43" s="18" t="n">
+        <v>44259</v>
+      </c>
       <c r="F43" s="31"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
@@ -29104,7 +29116,8 @@
     <hyperlink ref="F25" r:id="rId10" display="https://youtu.be/9zs9DaszFsc"/>
     <hyperlink ref="F36" r:id="rId11" display="https://youtu.be/tldgh05D1zc"/>
     <hyperlink ref="F37" r:id="rId12" display="https://youtu.be/B7X01IIgi8Q"/>
-    <hyperlink ref="F41" r:id="rId13" display="https://youtu.be/LPpOp21JWPk"/>
+    <hyperlink ref="F41" r:id="rId13" display="https://youtu.be/7muiM7fBkxY&#10;https://youtu.be/XjTfFqC4pks&#10;https://youtu.be/LPpOp21JWPk"/>
+    <hyperlink ref="F42" r:id="rId14" display="https://youtu.be/faEWkrmhco8"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #29 video record on youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t xml:space="preserve">Database #2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/D6hWp_krBFk </t>
   </si>
 </sst>
 </file>
@@ -708,8 +711,8 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F43" activeCellId="0" sqref="F43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F44" activeCellId="0" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2292,7 +2295,9 @@
       <c r="E43" s="18" t="n">
         <v>44259</v>
       </c>
-      <c r="F43" s="31"/>
+      <c r="F43" s="31" t="s">
+        <v>81</v>
+      </c>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
@@ -29118,6 +29123,7 @@
     <hyperlink ref="F37" r:id="rId12" display="https://youtu.be/B7X01IIgi8Q"/>
     <hyperlink ref="F41" r:id="rId13" display="https://youtu.be/7muiM7fBkxY&#10;https://youtu.be/XjTfFqC4pks&#10;https://youtu.be/LPpOp21JWPk"/>
     <hyperlink ref="F42" r:id="rId14" display="https://youtu.be/faEWkrmhco8"/>
+    <hyperlink ref="F43" r:id="rId15" display="https://youtu.be/D6hWp_krBFk"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #37 video record is in youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="99">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -337,6 +337,15 @@
   </si>
   <si>
     <t xml:space="preserve">https://youtu.be/mXr1kRr5NpA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Web development #2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/TN9Vuc1fRec </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Server, Servlet</t>
   </si>
 </sst>
 </file>
@@ -791,10 +800,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F54" activeCellId="0" sqref="F54"/>
+      <selection pane="topLeft" activeCell="F55" activeCellId="0" sqref="F55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -2700,12 +2709,18 @@
       <c r="B52" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="C52" s="21"/>
+      <c r="C52" s="21" t="s">
+        <v>96</v>
+      </c>
       <c r="D52" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="E52" s="18"/>
-      <c r="F52" s="35"/>
+      <c r="E52" s="18" t="n">
+        <v>44303</v>
+      </c>
+      <c r="F52" s="35" t="s">
+        <v>97</v>
+      </c>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
@@ -2732,11 +2747,15 @@
       <c r="B53" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C53" s="21"/>
+      <c r="C53" s="21" t="s">
+        <v>98</v>
+      </c>
       <c r="D53" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="E53" s="18"/>
+      <c r="E53" s="18" t="n">
+        <v>44305</v>
+      </c>
       <c r="F53" s="33"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
@@ -29314,7 +29333,8 @@
     <hyperlink ref="F47" r:id="rId18" display="https://youtu.be/-osnj3oh4jA"/>
     <hyperlink ref="F49" r:id="rId19" display="https://youtu.be/1xYX7pJqH54"/>
     <hyperlink ref="F50" r:id="rId20" display="https://youtu.be/jcUOEEm7abw "/>
-    <hyperlink ref="F51" r:id="rId21" display="https://youtu.be/mXr1kRr5NpA"/>
+    <hyperlink ref="F51" r:id="rId21" display="https://youtu.be/mXr1kRr5NpA "/>
+    <hyperlink ref="F52" r:id="rId22" display="https://youtu.be/TN9Vuc1fRec"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson 39 video record on youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="105">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -348,19 +348,22 @@
     <t xml:space="preserve">Server, Servlet</t>
   </si>
   <si>
-    <t xml:space="preserve">https://youtu.be/ohLgm-t0AFI</t>
+    <t xml:space="preserve">https://youtu.be/ohLgm-t0AFI </t>
   </si>
   <si>
     <t xml:space="preserve">Dynamic and Static Servlets</t>
   </si>
   <si>
-    <t xml:space="preserve">https://youtu.be/1GVb7YM8Wt8</t>
+    <t xml:space="preserve">https://youtu.be/1GVb7YM8Wt8 </t>
   </si>
   <si>
     <t xml:space="preserve">Freemarker</t>
   </si>
   <si>
     <t xml:space="preserve">REST </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web project in Java EE</t>
   </si>
 </sst>
 </file>
@@ -810,8 +813,8 @@
   </sheetPr>
   <dimension ref="A1:Z248"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C56" activeCellId="0" sqref="C56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C57" activeCellId="0" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2841,7 +2844,9 @@
       <c r="D55" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="E55" s="18"/>
+      <c r="E55" s="18" t="n">
+        <v>44312</v>
+      </c>
       <c r="F55" s="15"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
@@ -2867,7 +2872,7 @@
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="4"/>
       <c r="B56" s="11" t="n">
-        <v>8</v>
+        <v>8.1</v>
       </c>
       <c r="C56" s="21" t="s">
         <v>103</v>
@@ -2875,7 +2880,9 @@
       <c r="D56" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="E56" s="18"/>
+      <c r="E56" s="18" t="n">
+        <v>44314</v>
+      </c>
       <c r="F56" s="34"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
@@ -2898,7 +2905,21 @@
       <c r="Y56" s="4"/>
       <c r="Z56" s="4"/>
     </row>
-    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B57" s="11" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D57" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E57" s="18" t="n">
+        <v>44317</v>
+      </c>
+      <c r="F57" s="34"/>
+    </row>
     <row r="248" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="249" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="250" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3681,6 +3702,8 @@
     <hyperlink ref="F50" r:id="rId20" display="https://youtu.be/jcUOEEm7abw "/>
     <hyperlink ref="F51" r:id="rId21" display="https://youtu.be/mXr1kRr5NpA "/>
     <hyperlink ref="F52" r:id="rId22" display="https://youtu.be/TN9Vuc1fRec "/>
+    <hyperlink ref="F53" r:id="rId23" display="https://youtu.be/ohLgm-t0AFI"/>
+    <hyperlink ref="F54" r:id="rId24" display="https://youtu.be/1GVb7YM8Wt8"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson 40 video record on youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -814,7 +814,7 @@
   <dimension ref="A1:Z248"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C57" activeCellId="0" sqref="C57"/>
+      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3702,8 +3702,8 @@
     <hyperlink ref="F50" r:id="rId20" display="https://youtu.be/jcUOEEm7abw "/>
     <hyperlink ref="F51" r:id="rId21" display="https://youtu.be/mXr1kRr5NpA "/>
     <hyperlink ref="F52" r:id="rId22" display="https://youtu.be/TN9Vuc1fRec "/>
-    <hyperlink ref="F53" r:id="rId23" display="https://youtu.be/ohLgm-t0AFI"/>
-    <hyperlink ref="F54" r:id="rId24" display="https://youtu.be/1GVb7YM8Wt8"/>
+    <hyperlink ref="F53" r:id="rId23" display="https://youtu.be/ohLgm-t0AFI "/>
+    <hyperlink ref="F54" r:id="rId24" display="https://youtu.be/1GVb7YM8Wt8 "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #40 video record is in youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="106">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -358,6 +358,11 @@
   </si>
   <si>
     <t xml:space="preserve">Freemarker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/Ydrm-peBy7c
+https://youtu.be/JDTPdmMuNx0
+https://youtu.be/Rcj5HkzA8a4</t>
   </si>
   <si>
     <t xml:space="preserve">REST </t>
@@ -372,7 +377,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="D\-MMM\-YYYY"/>
+    <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
   </numFmts>
   <fonts count="18">
     <font>
@@ -736,12 +741,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -811,13 +816,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z248"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
+      <selection pane="topLeft" activeCell="E66" activeCellId="0" sqref="E66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -826,7 +831,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="61.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="7.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="12.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2833,7 +2837,7 @@
       <c r="Y54" s="4"/>
       <c r="Z54" s="4"/>
     </row>
-    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="41.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4"/>
       <c r="B55" s="13" t="n">
         <v>7</v>
@@ -2847,7 +2851,9 @@
       <c r="E55" s="18" t="n">
         <v>44312</v>
       </c>
-      <c r="F55" s="15"/>
+      <c r="F55" s="32" t="s">
+        <v>103</v>
+      </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
@@ -2875,7 +2881,7 @@
         <v>8.1</v>
       </c>
       <c r="C56" s="21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D56" s="13" t="n">
         <v>2</v>
@@ -2910,7 +2916,7 @@
         <v>8.2</v>
       </c>
       <c r="C57" s="21" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D57" s="13" t="n">
         <v>2</v>
@@ -3704,6 +3710,7 @@
     <hyperlink ref="F52" r:id="rId22" display="https://youtu.be/TN9Vuc1fRec "/>
     <hyperlink ref="F53" r:id="rId23" display="https://youtu.be/ohLgm-t0AFI "/>
     <hyperlink ref="F54" r:id="rId24" display="https://youtu.be/1GVb7YM8Wt8 "/>
+    <hyperlink ref="F55" r:id="rId25" display="https://youtu.be/Rcj5HkzA8a4"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #41 and #42 video records is in youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="109">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -360,15 +360,27 @@
     <t xml:space="preserve">Freemarker</t>
   </si>
   <si>
-    <t xml:space="preserve">https://youtu.be/Ydrm-peBy7c
-https://youtu.be/JDTPdmMuNx0
-https://youtu.be/Rcj5HkzA8a4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REST </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Web project in Java EE</t>
+    <t xml:space="preserve">1. https://youtu.be/Ydrm-peBy7c 
+2. https://youtu.be/JDTPdmMuNx0 
+3. https://youtu.be/Rcj5HkzA8a4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">REST (Json, XML)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. https://youtu.be/wNYuN-5TcCk 
+2. https://youtu.be/2VSN0CZhTJE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web project in Java EE – Part #1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. https://youtu.be/q1a3CS49zHE 
+2. https://youtu.be/6G_fIVU4VKM 
+3. https://youtu.be/jhAcrXZHab0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web project in Java EE – Part #2</t>
   </si>
 </sst>
 </file>
@@ -816,13 +828,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E66" activeCellId="0" sqref="E66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F58" activeCellId="0" sqref="F58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -2875,7 +2887,7 @@
       <c r="Y55" s="4"/>
       <c r="Z55" s="4"/>
     </row>
-    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4"/>
       <c r="B56" s="11" t="n">
         <v>8.1</v>
@@ -2887,9 +2899,11 @@
         <v>2</v>
       </c>
       <c r="E56" s="18" t="n">
-        <v>44314</v>
-      </c>
-      <c r="F56" s="34"/>
+        <v>44317</v>
+      </c>
+      <c r="F56" s="33" t="s">
+        <v>105</v>
+      </c>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
@@ -2911,21 +2925,104 @@
       <c r="Y56" s="4"/>
       <c r="Z56" s="4"/>
     </row>
-    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B57" s="11" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="C57" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="D57" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="E57" s="18" t="n">
-        <v>44317</v>
-      </c>
-      <c r="F57" s="34"/>
-    </row>
+    <row r="58" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C58" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="D58" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E58" s="18" t="n">
+        <v>44319</v>
+      </c>
+      <c r="F58" s="33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D59" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E59" s="18"/>
+      <c r="F59" s="35"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="13" t="n">
+        <v>3</v>
+      </c>
+      <c r="C60" s="21"/>
+      <c r="D60" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E60" s="18"/>
+      <c r="F60" s="35"/>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="C61" s="21"/>
+      <c r="D61" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E61" s="18"/>
+      <c r="F61" s="35"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="C62" s="21"/>
+      <c r="D62" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E62" s="18"/>
+      <c r="F62" s="33"/>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="C63" s="21"/>
+      <c r="D63" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E63" s="18"/>
+      <c r="F63" s="33"/>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="13" t="n">
+        <v>7</v>
+      </c>
+      <c r="C64" s="21"/>
+      <c r="D64" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E64" s="18"/>
+      <c r="F64" s="32"/>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="C65" s="21"/>
+      <c r="D65" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E65" s="18"/>
+      <c r="F65" s="34"/>
+    </row>
+    <row r="246" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="247" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="248" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="249" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="250" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3677,8 +3774,8 @@
     <row r="996" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="997" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="998" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="999" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1000" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A4:A11"/>
@@ -3710,7 +3807,6 @@
     <hyperlink ref="F52" r:id="rId22" display="https://youtu.be/TN9Vuc1fRec "/>
     <hyperlink ref="F53" r:id="rId23" display="https://youtu.be/ohLgm-t0AFI "/>
     <hyperlink ref="F54" r:id="rId24" display="https://youtu.be/1GVb7YM8Wt8 "/>
-    <hyperlink ref="F55" r:id="rId25" display="https://youtu.be/Rcj5HkzA8a4"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson 43 video record on youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -389,7 +389,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
+    <numFmt numFmtId="165" formatCode="D\-MMM\-YYYY"/>
   </numFmts>
   <fonts count="18">
     <font>
@@ -753,12 +753,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -830,11 +830,11 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F58" activeCellId="0" sqref="F58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F59" activeCellId="0" sqref="F59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -843,6 +843,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="61.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="7.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="12.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2952,7 +2953,9 @@
       <c r="D59" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="E59" s="18"/>
+      <c r="E59" s="18" t="n">
+        <v>44322</v>
+      </c>
       <c r="F59" s="35"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
lesson 44 topic added
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="112">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -386,6 +386,15 @@
     <t xml:space="preserve">1. https://youtu.be/i0XnA0d_kEk
 2. https://youtu.be/wu2YbqPoVEM
 3. https://youtu.be/QhPz6cun3zc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web project in Java EE – Part #3 
+– DEPLOY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. https://youtu.be/e0QbixUZ3fM 
+2. https://youtu.be/fuNIo6ZFj5k 
+3. https://youtu.be/4Bgxq_bi23E </t>
   </si>
 </sst>
 </file>
@@ -611,7 +620,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -756,6 +765,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -836,7 +849,7 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B57" activeCellId="0" sqref="B57"/>
+      <selection pane="topLeft" activeCell="F60" activeCellId="0" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2948,7 +2961,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="41.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="13" t="n">
         <v>2</v>
       </c>
@@ -2965,16 +2978,22 @@
         <v>109</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="41.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="C60" s="21"/>
+      <c r="C60" s="36" t="s">
+        <v>110</v>
+      </c>
       <c r="D60" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="E60" s="18"/>
-      <c r="F60" s="35"/>
+      <c r="E60" s="18" t="n">
+        <v>44326</v>
+      </c>
+      <c r="F60" s="35" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="13" t="n">
@@ -3817,6 +3836,7 @@
     <hyperlink ref="F52" r:id="rId22" display="https://youtu.be/TN9Vuc1fRec "/>
     <hyperlink ref="F53" r:id="rId23" display="https://youtu.be/ohLgm-t0AFI "/>
     <hyperlink ref="F54" r:id="rId24" display="https://youtu.be/1GVb7YM8Wt8 "/>
+    <hyperlink ref="F60" r:id="rId25" display="https://youtu.be/e0QbixUZ3fM"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson ##45 video records is in youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -403,7 +403,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="D\-MMM\-YYYY"/>
+    <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
   </numFmts>
   <fonts count="18">
     <font>
@@ -771,12 +771,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -849,10 +849,10 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F60" activeCellId="0" sqref="F60"/>
+      <selection pane="topLeft" activeCell="E69" activeCellId="0" sqref="E69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -861,7 +861,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="61.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="7.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="12.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3049,6 +3048,17 @@
       </c>
       <c r="E65" s="18"/>
       <c r="F65" s="34"/>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C66" s="21"/>
+      <c r="D66" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E66" s="18"/>
+      <c r="F66" s="34"/>
     </row>
     <row r="246" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="247" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3836,7 +3846,7 @@
     <hyperlink ref="F52" r:id="rId22" display="https://youtu.be/TN9Vuc1fRec "/>
     <hyperlink ref="F53" r:id="rId23" display="https://youtu.be/ohLgm-t0AFI "/>
     <hyperlink ref="F54" r:id="rId24" display="https://youtu.be/1GVb7YM8Wt8 "/>
-    <hyperlink ref="F60" r:id="rId25" display="https://youtu.be/e0QbixUZ3fM"/>
+    <hyperlink ref="F60" r:id="rId25" display="1. https://youtu.be/e0QbixUZ3fM &#10;2. https://youtu.be/fuNIo6ZFj5k &#10;3. https://youtu.be/4Bgxq_bi23E "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson ##46 video record on uploaded
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="116">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -401,6 +401,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://youtu.be/Iik3L8Eodg4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IoC and DI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/8eHrHZtqum8</t>
   </si>
 </sst>
 </file>
@@ -855,10 +861,10 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E62" activeCellId="0" sqref="E62"/>
+      <selection pane="topLeft" activeCell="C68" activeCellId="0" sqref="C68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -3000,7 +3006,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="13" t="n">
         <v>4</v>
       </c>
@@ -3017,16 +3023,22 @@
         <v>113</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C62" s="21"/>
+      <c r="C62" s="21" t="s">
+        <v>114</v>
+      </c>
       <c r="D62" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="E62" s="18"/>
-      <c r="F62" s="33"/>
+      <c r="E62" s="18" t="n">
+        <v>44337</v>
+      </c>
+      <c r="F62" s="33" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="13" t="n">
@@ -3061,17 +3073,7 @@
       <c r="E65" s="18"/>
       <c r="F65" s="34"/>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="11" t="n">
-        <v>9</v>
-      </c>
-      <c r="C66" s="21"/>
-      <c r="D66" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="E66" s="18"/>
-      <c r="F66" s="34"/>
-    </row>
+    <row r="245" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="246" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="247" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="248" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3824,7 +3826,7 @@
     <row r="995" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="996" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="997" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="998" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
lesson ##47 video record on uploaded
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="118">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -403,10 +403,16 @@
     <t xml:space="preserve">https://youtu.be/Iik3L8Eodg4</t>
   </si>
   <si>
-    <t xml:space="preserve">IoC and DI</t>
+    <t xml:space="preserve">IoC and DI, Thymeleaf</t>
   </si>
   <si>
     <t xml:space="preserve">https://youtu.be/8eHrHZtqum8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring Rest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/I9qweBBYzzE</t>
   </si>
 </sst>
 </file>
@@ -861,10 +867,10 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C68" activeCellId="0" sqref="C68"/>
+      <selection pane="topLeft" activeCell="E65" activeCellId="0" sqref="E65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -3040,16 +3046,22 @@
         <v>115</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="C63" s="21"/>
+      <c r="C63" s="21" t="s">
+        <v>116</v>
+      </c>
       <c r="D63" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="E63" s="18"/>
-      <c r="F63" s="33"/>
+      <c r="E63" s="18" t="n">
+        <v>44341</v>
+      </c>
+      <c r="F63" s="33" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="13" t="n">

</xml_diff>

<commit_message>
course syllabus changed a bit
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="122">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -413,6 +413,36 @@
   </si>
   <si>
     <t xml:space="preserve">https://youtu.be/I9qweBBYzzE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring web project intro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/sUR7FrS99BQ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring Data Jpa – Hibernate, H2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Bonus – Deployment, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Intern/Job application</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -421,9 +451,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
+    <numFmt numFmtId="165" formatCode="D\-MMM\-YYYY"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -555,8 +585,14 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -566,13 +602,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFF200"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -638,7 +680,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -787,14 +829,18 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -824,7 +870,7 @@
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
@@ -866,19 +912,20 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E65" activeCellId="0" sqref="E65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F65" activeCellId="0" sqref="F65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="61.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="7.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="12.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3063,27 +3110,52 @@
         <v>117</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="C64" s="21"/>
+      <c r="C64" s="0" t="s">
+        <v>118</v>
+      </c>
       <c r="D64" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="E64" s="18"/>
-      <c r="F64" s="32"/>
+      <c r="E64" s="18" t="n">
+        <v>44342</v>
+      </c>
+      <c r="F64" s="32" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="11" t="n">
+      <c r="B65" s="37" t="n">
         <v>8</v>
       </c>
-      <c r="C65" s="21"/>
+      <c r="C65" s="21" t="s">
+        <v>120</v>
+      </c>
       <c r="D65" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="E65" s="18"/>
-      <c r="F65" s="34"/>
+      <c r="E65" s="18" t="n">
+        <v>44345</v>
+      </c>
+      <c r="F65" s="32"/>
+    </row>
+    <row r="66" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C66" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D66" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E66" s="18" t="n">
+        <v>44349</v>
+      </c>
+      <c r="F66" s="34"/>
     </row>
     <row r="245" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="246" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3873,6 +3945,7 @@
     <hyperlink ref="F53" r:id="rId23" display="https://youtu.be/ohLgm-t0AFI "/>
     <hyperlink ref="F54" r:id="rId24" display="https://youtu.be/1GVb7YM8Wt8 "/>
     <hyperlink ref="F60" r:id="rId25" display="1. https://youtu.be/e0QbixUZ3fM &#10;2. https://youtu.be/fuNIo6ZFj5k &#10;3. https://youtu.be/4Bgxq_bi23E "/>
+    <hyperlink ref="F64" r:id="rId26" display="https://youtu.be/sUR7FrS99BQ "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #49 video record on uploaded
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="123">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -424,25 +424,11 @@
     <t xml:space="preserve">Spring Data Jpa – Hibernate, H2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Bonus – Deployment, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Intern/Job application</t>
-    </r>
+    <t xml:space="preserve">1. https://youtu.be/t7IrVajlsGg
+2. https://youtu.be/LF-btusPJbw </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonus – Deployment, Intern/Job application</t>
   </si>
 </sst>
 </file>
@@ -451,9 +437,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="D\-MMM\-YYYY"/>
+    <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -584,12 +570,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="5">
@@ -835,12 +815,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -913,10 +893,10 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F65" activeCellId="0" sqref="F65"/>
+      <selection pane="topLeft" activeCell="F72" activeCellId="0" sqref="F72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55078125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
@@ -925,7 +905,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="61.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="7.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="12.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3127,7 +3106,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="37" t="n">
         <v>8</v>
       </c>
@@ -3140,14 +3119,16 @@
       <c r="E65" s="18" t="n">
         <v>44345</v>
       </c>
-      <c r="F65" s="32"/>
+      <c r="F65" s="32" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="11" t="n">
         <v>9</v>
       </c>
       <c r="C66" s="21" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D66" s="13" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
lesson #50 video record on uploaded
</commit_message>
<xml_diff>
--- a/src/main/java/org/course/_syllabus/course_details.xlsx
+++ b/src/main/java/org/course/_syllabus/course_details.xlsx
@@ -421,7 +421,7 @@
     <t xml:space="preserve">https://youtu.be/sUR7FrS99BQ </t>
   </si>
   <si>
-    <t xml:space="preserve">Spring Data Jpa – Hibernate, H2</t>
+    <t xml:space="preserve">Spring Data Jpa – Hibernate, H2, PostgreSQL</t>
   </si>
   <si>
     <t xml:space="preserve">1. https://youtu.be/t7IrVajlsGg
@@ -892,15 +892,15 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F72" activeCellId="0" sqref="F72"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C66" activeCellId="0" sqref="C66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.55078125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="61.62"/>

</xml_diff>